<commit_message>
Fixed failure scripts - Vacc & eCare. Updated Docker related files
</commit_message>
<xml_diff>
--- a/ExcelTestReport.xlsx
+++ b/ExcelTestReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="74">
   <si>
     <t>Test Step #</t>
   </si>
@@ -25,15 +25,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Start Time</t>
-  </si>
-  <si>
-    <t>End Time</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Step 1</t>
   </si>
   <si>
@@ -70,13 +61,13 @@
     <t>Step 5a</t>
   </si>
   <si>
-    <t xml:space="preserve"> Firstname:TestAutomation73143</t>
+    <t xml:space="preserve"> Firstname:TestAutomation6840</t>
   </si>
   <si>
     <t>Step 5b</t>
   </si>
   <si>
-    <t xml:space="preserve"> Lastname:User41142</t>
+    <t xml:space="preserve"> Lastname:User92986</t>
   </si>
   <si>
     <t>Step 5c</t>
@@ -226,10 +217,10 @@
     <t xml:space="preserve"> Clicked Completed Link </t>
   </si>
   <si>
-    <t xml:space="preserve"> Firstname:TestAutomation55829</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lastname:User93797</t>
+    <t xml:space="preserve"> Firstname:TestAutomation48623</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lastname:User4558</t>
   </si>
   <si>
     <t xml:space="preserve"> Clicked Vaccination Tab </t>
@@ -242,6 +233,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Validated Vaccine Administered message </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validated Vaccine History Section for added vaccination </t>
   </si>
 </sst>
 </file>
@@ -618,16 +612,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:C29"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -637,316 +630,307 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -957,16 +941,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:C4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -976,41 +959,32 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1021,16 +995,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:C13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1040,140 +1013,131 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1184,16 +1148,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:C22"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="6" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1203,228 +1166,230 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Custom Excel Report
</commit_message>
<xml_diff>
--- a/ExcelTestReport.xlsx
+++ b/ExcelTestReport.xlsx
@@ -3,18 +3,110 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <sheets>
+    <sheet sheetId="1" name="Negative_Scenario" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="OnDemand_POC" state="visible" r:id="rId5"/>
+  </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+  <si>
+    <t>Test Step #</t>
+  </si>
+  <si>
+    <t>Test Step Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Entered User Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Passed</t>
+  </si>
+  <si>
+    <t>Step 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Entered Password </t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Script Failed at Step #3</t>
+  </si>
+  <si>
+    <t>Step 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clicked SignIn Btn </t>
+  </si>
+  <si>
+    <t>Step 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clicked Active Patient </t>
+  </si>
+  <si>
+    <t>Step 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Selected First Patient </t>
+  </si>
+  <si>
+    <t>Step 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clicked On Demand under Action Menu </t>
+  </si>
+  <si>
+    <t>Step 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clicked On Demand Campaign </t>
+  </si>
+  <si>
+    <t>Step 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clicked Send Message Button </t>
+  </si>
+  <si>
+    <t>Step 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validated Success Message </t>
+  </si>
+  <si>
+    <t>Script Failed at Step #10</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u val="double"/>
+      <color rgb="E70B0B"/>
+      <family val="4"/>
+      <sz val="15"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -38,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,4 +468,199 @@
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>